<commit_message>
Update Excel template again
</commit_message>
<xml_diff>
--- a/public/人口登记表-zhCn.xlsx
+++ b/public/人口登记表-zhCn.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
   <si>
     <t>uid</t>
   </si>
@@ -50,7 +50,7 @@
     <t>未来已到</t>
   </si>
   <si>
-    <t>https://pub-8d9c7b440bdc4316a94cd1a6ec45d0ce.r2.dev/%E5%A4%B4%E5%83%8F/%E5%A4%B4%E5%83%8F.jpg</t>
+    <t>https://img1.baidu.com/it/u=2165937980,813753762&amp;fm=253&amp;fmt=auto&amp;app=138&amp;f=JPEG?w=500&amp;h=500</t>
   </si>
   <si>
     <t>801</t>
@@ -65,9 +65,6 @@
     <t>长毛</t>
   </si>
   <si>
-    <t>https://pub-8d9c7b440bdc4316a94cd1a6ec45d0ce.r2.dev/%E5%A4%B4%E5%83%8F/Generated%20Image%20March%2028%2C%202025%20-%2011_04PM.jpeg</t>
-  </si>
-  <si>
     <t>主任</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>锅盖</t>
   </si>
   <si>
-    <t>https://pub-8d9c7b440bdc4316a94cd1a6ec45d0ce.r2.dev/%E5%A4%B4%E5%83%8F/Generated%20Image%20March%2028%2C%202025%20-%2011_17PM.jpeg</t>
-  </si>
-  <si>
     <t>老师</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>卷毛</t>
   </si>
   <si>
-    <t>https://pub-8d9c7b440bdc4316a94cd1a6ec45d0ce.r2.dev/%E5%A4%B4%E5%83%8F/Generated%20Image%20March%2030%2C%202025%20-%208_49PM.jpeg</t>
-  </si>
-  <si>
     <t>班长</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>肥仔</t>
   </si>
   <si>
-    <t>https://pub-8d9c7b440bdc4316a94cd1a6ec45d0ce.r2.dev/%E5%A4%B4%E5%83%8F/Generated%20Image%20March%2030%2C%202025%20-%208_51PM.jpeg</t>
-  </si>
-  <si>
     <t>组长</t>
   </si>
   <si>
@@ -111,9 +99,6 @@
   </si>
   <si>
     <t>张居正</t>
-  </si>
-  <si>
-    <t>https://img1.baidu.com/it/u=2165937980,813753762&amp;fm=253&amp;fmt=auto&amp;app=138&amp;f=JPEG?w=500&amp;h=500</t>
   </si>
   <si>
     <t>学生</t>
@@ -318,24 +303,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -772,28 +757,28 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -917,9 +902,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1313,7 +1297,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.64285714285714" defaultRowHeight="17.6" outlineLevelCol="4"/>
@@ -1365,602 +1349,599 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D15" t="s">
         <v>8</v>
       </c>
       <c r="E15" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D16" t="s">
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D17" t="s">
         <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>8</v>
       </c>
       <c r="E18" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D19" t="s">
         <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
         <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
         <v>8</v>
       </c>
       <c r="E22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
         <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
         <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D25" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
         <v>8</v>
       </c>
       <c r="E26" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D27" t="s">
         <v>8</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B29" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B30" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D31" t="s">
         <v>8</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D32" t="s">
         <v>8</v>
       </c>
       <c r="E32" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D33" t="s">
         <v>8</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B34" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D34" t="s">
         <v>8</v>
       </c>
       <c r="E34" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D35" t="s">
         <v>8</v>
       </c>
       <c r="E35" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D36" t="s">
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
         <v>8</v>
       </c>
       <c r="E37" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" display="https://pub-8d9c7b440bdc4316a94cd1a6ec45d0ce.r2.dev/%E5%A4%B4%E5%83%8F/Generated%20Image%20March%2028%2C%202025%20-%2011_04PM.jpeg"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <ignoredErrors>
-    <ignoredError sqref="A1:E1 A2:A6 D2:D6 A7:E37" numberStoredAsText="1"/>
+    <ignoredError sqref="A7:B7 D7:E7 A8:E37 D2:D6 A2:A6 A1:E1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>